<commit_message>
Added MySQL dynamic query for variable rows number
</commit_message>
<xml_diff>
--- a/xls.xlsx
+++ b/xls.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="2">
   <si>
     <t>abc</t>
   </si>
@@ -360,147 +360,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D2" sqref="A2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>42645</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>42645</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>42646</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42646</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>42647</v>
       </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42647</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>42648</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>42648</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>42649</v>
       </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42649</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>42650</v>
       </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>42650</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>42651</v>
       </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>42651</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>42652</v>
       </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>42652</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>42653</v>
       </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1">
+        <v>42653</v>
+      </c>
+      <c r="F10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>42654</v>
       </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
+        <v>42654</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>42655</v>
       </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1">
+        <v>42655</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>42656</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1">
+        <v>42656</v>
+      </c>
+      <c r="F13" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
JS: a lot rewrites, PHP: cleaned empty rows from the query
</commit_message>
<xml_diff>
--- a/xls.xlsx
+++ b/xls.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="3">
   <si>
     <t>abc</t>
   </si>
   <si>
     <t>דגכדגכ גכדגכ</t>
+  </si>
+  <si>
+    <t>דגכדגכ</t>
   </si>
 </sst>
 </file>
@@ -362,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:F13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +393,7 @@
         <v>42645</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -410,7 +413,7 @@
         <v>42646</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -430,7 +433,7 @@
         <v>42647</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -450,7 +453,7 @@
         <v>42648</v>
       </c>
       <c r="F5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -470,7 +473,7 @@
         <v>42649</v>
       </c>
       <c r="F6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -490,7 +493,7 @@
         <v>42650</v>
       </c>
       <c r="F7" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -510,7 +513,7 @@
         <v>42651</v>
       </c>
       <c r="F8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -530,7 +533,7 @@
         <v>42652</v>
       </c>
       <c r="F9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -550,7 +553,7 @@
         <v>42653</v>
       </c>
       <c r="F10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -570,7 +573,7 @@
         <v>42654</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>